<commit_message>
Criando as planilhas e importando a planilha com openpyxl
</commit_message>
<xml_diff>
--- a/files/chart.xlsx
+++ b/files/chart.xlsx
@@ -1,34 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\Recursos\Documents\Programação\Python\Módulo 6\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EE4E12-B3F7-48DA-8C9C-C5309F6202B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Lucro</t>
+  </si>
+  <si>
+    <t>Custos</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,233 +65,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="12"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="112"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="12"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="pt-BR"/>
               <a:t>Lucro x Custos por Ano</a:t>
             </a:r>
           </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <areaChart>
-        <grouping val="standard"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <spPr>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Sheet'!$A$1:$A$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Sheet'!$B$1:$B$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <spPr>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Ano</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD88-4449-AC82-4A192842D707}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
             <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Sheet'!$A$1:$A$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Sheet'!$C$1:$C$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <axId val="10"/>
-        <axId val="100"/>
-      </areaChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Ano</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$C$1:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BD88-4449-AC82-4A192842D707}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="10"/>
+        <c:axId val="100"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="10"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="pt-BR"/>
                   <a:t>Ano</a:t>
                 </a:r>
               </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="100"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
               <a:bodyPr/>
+              <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="pt-BR"/>
                   <a:t>Porcentagem</a:t>
                 </a:r>
               </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="10"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,99 +685,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Ano</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Lucro</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Custos</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2017</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>40</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>30</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2018</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>35</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>25</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2019</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>20</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2020</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2021</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>15</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2022</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>25</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>15</v>
       </c>
     </row>

</xml_diff>